<commit_message>
Manage News Update, Admin User, Manage Footer Text, Manage Footer Text Validation, Add Category
</commit_message>
<xml_diff>
--- a/7RMartSupermarket/src/test/resources/testdata.xlsx
+++ b/7RMartSupermarket/src/test/resources/testdata.xlsx
@@ -5,17 +5,20 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acer\eclipse-workspace\7RMartSupermarket\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acer\git\7RMartSupermarket\7RMartSupermarket\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C750EAE-3F91-4E19-85BD-6B41480D17AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAE99DCC-0053-4B96-905B-596118D294C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1060" yWindow="1060" windowWidth="14400" windowHeight="7360" activeTab="2" xr2:uid="{2D5A69A1-993C-4B18-85CA-817525B0367F}"/>
+    <workbookView xWindow="1060" yWindow="1060" windowWidth="14400" windowHeight="7360" firstSheet="2" activeTab="4" xr2:uid="{2D5A69A1-993C-4B18-85CA-817525B0367F}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPage" sheetId="1" r:id="rId1"/>
     <sheet name="ManageNewsPage" sheetId="2" r:id="rId2"/>
-    <sheet name="ManageContactPage" sheetId="3" r:id="rId3"/>
+    <sheet name="ManageFooterTextPage" sheetId="4" r:id="rId3"/>
+    <sheet name="ManageCategory" sheetId="5" r:id="rId4"/>
+    <sheet name="AdminUsers" sheetId="6" r:id="rId5"/>
+    <sheet name="ManageContactPage" sheetId="3" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="23">
   <si>
     <t>username</t>
   </si>
@@ -57,6 +60,45 @@
   </si>
   <si>
     <t>Flat No 123</t>
+  </si>
+  <si>
+    <t>Hello, Welcome to Coding!!</t>
+  </si>
+  <si>
+    <t>Footer Text Informations</t>
+  </si>
+  <si>
+    <t>Fno: 1234, Skyline, Kerala</t>
+  </si>
+  <si>
+    <t>0485 227221</t>
+  </si>
+  <si>
+    <t>skyline@yopmail.com</t>
+  </si>
+  <si>
+    <t>Add Cattegory</t>
+  </si>
+  <si>
+    <t>Pizza1</t>
+  </si>
+  <si>
+    <t>Credentials</t>
+  </si>
+  <si>
+    <t>teststaff123</t>
+  </si>
+  <si>
+    <t>teststaff1</t>
+  </si>
+  <si>
+    <t>testadmin</t>
+  </si>
+  <si>
+    <t>testpartner</t>
+  </si>
+  <si>
+    <t>testdb</t>
   </si>
 </sst>
 </file>
@@ -474,22 +516,88 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E16E90C-C68E-4AFF-A17A-A2B7E29F4036}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4610D0D3-F177-4466-B317-A091AC9E2D50}">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A3" r:id="rId1" xr:uid="{AE208F98-ADE0-46E0-B4A2-D0A80F085182}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58EF7F42-A67C-4ED1-B833-19DD85A3F1B9}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -497,11 +605,63 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C648BD6D-2C40-4C4B-95B0-086386E21719}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3551CA62-AB7F-4792-9E68-158716748247}">
   <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Adding MultiBrowser Testing, Cross Browser Testing, Parallel Testing scripts
</commit_message>
<xml_diff>
--- a/7RMartSupermarket/src/test/resources/testdata.xlsx
+++ b/7RMartSupermarket/src/test/resources/testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acer\git\7RMartSupermarket\7RMartSupermarket\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAE99DCC-0053-4B96-905B-596118D294C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E102A752-B449-40B1-A9DA-8D93C196263B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1060" yWindow="1060" windowWidth="14400" windowHeight="7360" firstSheet="2" activeTab="4" xr2:uid="{2D5A69A1-993C-4B18-85CA-817525B0367F}"/>
+    <workbookView xWindow="1060" yWindow="1060" windowWidth="14400" windowHeight="7360" firstSheet="2" activeTab="3" xr2:uid="{2D5A69A1-993C-4B18-85CA-817525B0367F}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPage" sheetId="1" r:id="rId1"/>
@@ -80,9 +80,6 @@
     <t>Add Cattegory</t>
   </si>
   <si>
-    <t>Pizza1</t>
-  </si>
-  <si>
     <t>Credentials</t>
   </si>
   <si>
@@ -99,6 +96,9 @@
   </si>
   <si>
     <t>testdb</t>
+  </si>
+  <si>
+    <t>Pizza L</t>
   </si>
 </sst>
 </file>
@@ -584,8 +584,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58EF7F42-A67C-4ED1-B833-19DD85A3F1B9}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -597,7 +597,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -609,7 +609,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C648BD6D-2C40-4C4B-95B0-086386E21719}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -617,39 +617,39 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
minor changes with jsclick method in PageUtilities
</commit_message>
<xml_diff>
--- a/7RMartSupermarket/src/test/resources/testdata.xlsx
+++ b/7RMartSupermarket/src/test/resources/testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acer\git\7RMartSupermarket\7RMartSupermarket\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E102A752-B449-40B1-A9DA-8D93C196263B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09B5EC2E-2595-47E3-8065-49D81F57854C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1060" yWindow="1060" windowWidth="14400" windowHeight="7360" firstSheet="2" activeTab="3" xr2:uid="{2D5A69A1-993C-4B18-85CA-817525B0367F}"/>
   </bookViews>
@@ -98,7 +98,7 @@
     <t>testdb</t>
   </si>
   <si>
-    <t>Pizza L</t>
+    <t>Pizza M</t>
   </si>
 </sst>
 </file>
@@ -585,7 +585,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
minor changes and new Testng file creation
</commit_message>
<xml_diff>
--- a/7RMartSupermarket/src/test/resources/testdata.xlsx
+++ b/7RMartSupermarket/src/test/resources/testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acer\git\7RMartSupermarket\7RMartSupermarket\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{390DA829-B9B7-4A1A-9AD1-3459ADA009D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4812467B-8ACD-45EA-8643-9B974C895476}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1060" yWindow="1060" windowWidth="14400" windowHeight="7360" xr2:uid="{2D5A69A1-993C-4B18-85CA-817525B0367F}"/>
+    <workbookView xWindow="1060" yWindow="1060" windowWidth="14400" windowHeight="7360" firstSheet="3" activeTab="5" xr2:uid="{2D5A69A1-993C-4B18-85CA-817525B0367F}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPage" sheetId="1" r:id="rId1"/>
@@ -56,9 +56,6 @@
     <t>Contact Details</t>
   </si>
   <si>
-    <t>Hello, Welcome to Coding!!</t>
-  </si>
-  <si>
     <t>Footer Text Informations</t>
   </si>
   <si>
@@ -86,19 +83,22 @@
     <t>testdb</t>
   </si>
   <si>
-    <t>Pizza XL</t>
-  </si>
-  <si>
     <t>testuser@yopmail.com</t>
   </si>
   <si>
     <t>Flat No 1207</t>
   </si>
   <si>
-    <t>Fno: 12B, Skyline, Kerala</t>
-  </si>
-  <si>
     <t>0485 2273222</t>
+  </si>
+  <si>
+    <t>Welcome to Coding!! JS</t>
+  </si>
+  <si>
+    <t>FNmbr: 1207B, Skyline Apart, Kerala</t>
+  </si>
+  <si>
+    <t>Pizza XS</t>
   </si>
 </sst>
 </file>
@@ -463,7 +463,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D91C88D-41A5-4434-A18A-1CECA3AF13A6}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
@@ -519,7 +519,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -534,7 +534,7 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -547,14 +547,14 @@
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
@@ -564,12 +564,12 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -585,19 +585,19 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -610,46 +610,46 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -661,7 +661,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3551CA62-AB7F-4792-9E68-158716748247}">
   <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -682,12 +682,12 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
latest changes with chaining feature
</commit_message>
<xml_diff>
--- a/7RMartSupermarket/src/test/resources/testdata.xlsx
+++ b/7RMartSupermarket/src/test/resources/testdata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acer\git\7RMartSupermarket\7RMartSupermarket\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4812467B-8ACD-45EA-8643-9B974C895476}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEC0696C-AA18-4559-BD79-451C4972C361}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1060" yWindow="1060" windowWidth="14400" windowHeight="7360" firstSheet="3" activeTab="5" xr2:uid="{2D5A69A1-993C-4B18-85CA-817525B0367F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="2" activeTab="5" xr2:uid="{2D5A69A1-993C-4B18-85CA-817525B0367F}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPage" sheetId="1" r:id="rId1"/>
@@ -47,12 +47,6 @@
     <t>Test</t>
   </si>
   <si>
-    <t>text</t>
-  </si>
-  <si>
-    <t>HelloWorld</t>
-  </si>
-  <si>
     <t>Contact Details</t>
   </si>
   <si>
@@ -80,25 +74,31 @@
     <t>testpartner</t>
   </si>
   <si>
-    <t>testdb</t>
-  </si>
-  <si>
     <t>testuser@yopmail.com</t>
   </si>
   <si>
-    <t>Flat No 1207</t>
-  </si>
-  <si>
-    <t>0485 2273222</t>
-  </si>
-  <si>
-    <t>Welcome to Coding!! JS</t>
-  </si>
-  <si>
-    <t>FNmbr: 1207B, Skyline Apart, Kerala</t>
-  </si>
-  <si>
-    <t>Pizza XS</t>
+    <t>Original Text</t>
+  </si>
+  <si>
+    <t>Updation Text</t>
+  </si>
+  <si>
+    <t>bunt</t>
+  </si>
+  <si>
+    <t>testdb2</t>
+  </si>
+  <si>
+    <t>Hello, Selenium Test</t>
+  </si>
+  <si>
+    <t>FNmbr: 1207B, Confident Atlenna</t>
+  </si>
+  <si>
+    <t>Flat No 1234</t>
+  </si>
+  <si>
+    <t>Hello, TestNG Test</t>
   </si>
 </sst>
 </file>
@@ -519,22 +519,29 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="23.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.54296875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -547,7 +554,48 @@
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="30.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>9876512345</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A3" r:id="rId1" xr:uid="{AE208F98-ADE0-46E0-B4A2-D0A80F085182}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58EF7F42-A67C-4ED1-B833-19DD85A3F1B9}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -559,30 +607,17 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A3" r:id="rId1" xr:uid="{AE208F98-ADE0-46E0-B4A2-D0A80F085182}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58EF7F42-A67C-4ED1-B833-19DD85A3F1B9}">
-  <dimension ref="A1:A2"/>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C648BD6D-2C40-4C4B-95B0-086386E21719}">
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
@@ -590,66 +625,41 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C648BD6D-2C40-4C4B-95B0-086386E21719}">
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -662,7 +672,7 @@
   <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -672,32 +682,32 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2">
-        <v>9876543210</v>
+        <v>9945995541</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5">
-        <v>25</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6">
-        <v>50</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changing method names for manage contact page class
</commit_message>
<xml_diff>
--- a/7RMartSupermarket/src/test/resources/testdata.xlsx
+++ b/7RMartSupermarket/src/test/resources/testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acer\git\7RMartSupermarket\7RMartSupermarket\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEC0696C-AA18-4559-BD79-451C4972C361}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5F72896-9AF8-4625-89CF-1B5D24F8EE7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="2" activeTab="5" xr2:uid="{2D5A69A1-993C-4B18-85CA-817525B0367F}"/>
   </bookViews>
@@ -74,9 +74,6 @@
     <t>testpartner</t>
   </si>
   <si>
-    <t>testuser@yopmail.com</t>
-  </si>
-  <si>
     <t>Original Text</t>
   </si>
   <si>
@@ -95,10 +92,13 @@
     <t>FNmbr: 1207B, Confident Atlenna</t>
   </si>
   <si>
-    <t>Flat No 1234</t>
-  </si>
-  <si>
     <t>Hello, TestNG Test</t>
+  </si>
+  <si>
+    <t>userdummy@yopmail.com</t>
+  </si>
+  <si>
+    <t>Flat No 1207A</t>
   </si>
 </sst>
 </file>
@@ -530,18 +530,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
         <v>15</v>
-      </c>
-      <c r="B1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -569,7 +569,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
@@ -607,7 +607,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -656,10 +656,10 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -672,12 +672,12 @@
   <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
@@ -687,27 +687,27 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2">
-        <v>9945995541</v>
+        <v>8281828182</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5">
-        <v>75</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6">
-        <v>15</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>